<commit_message>
Worked on the Operations section: 1
</commit_message>
<xml_diff>
--- a/Data/MAIN_DATA_FILE.xlsx
+++ b/Data/MAIN_DATA_FILE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jolantav\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andris\Desktop\PEI_LD4_Streamlit_Dash_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E93D0A-A20B-4355-8DC8-5EE95916D9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D447809B-BAD0-4A45-86E1-9D067B8AE267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="17640" tabRatio="914" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="914" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component" sheetId="2" r:id="rId1"/>
@@ -458,7 +458,7 @@
     <numFmt numFmtId="168" formatCode="#0.000"/>
     <numFmt numFmtId="169" formatCode="#0.00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -496,7 +496,7 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -800,9 +800,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -914,7 +914,7 @@
         <v>5857978</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -970,7 +970,7 @@
         <v>6059897</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>6059897</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>5708860</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>5952555</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>5585851</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>6040156</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>5611697</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>5611697</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>5259397</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>5716639</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>5318427</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>1389065</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>1420397</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>1420397</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>1326400</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>1423879</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>1314216</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>85322</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>76909</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>76909</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>74820</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>90516</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>73979</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>16087</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>14571</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>14571</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>14049</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>16543</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -2549,9 +2549,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2588,9 +2588,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>128</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>128</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>128</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>128</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>128</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>128</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>128</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>128</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>128</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>128</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>128</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>128</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>128</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>128</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>128</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>128</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>128</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>128</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>128</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>128</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>128</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>128</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>128</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>128</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>128</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>128</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>128</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>128</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>128</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>128</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>128</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>128</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>128</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>128</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>128</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>128</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>128</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>128</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>128</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>128</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>128</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>128</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>128</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>128</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>128</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>128</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>128</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>128</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>128</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>128</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>128</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>128</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>128</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>128</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>128</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>128</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>128</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>128</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>128</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>128</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>128</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>128</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>128</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>128</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>128</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>128</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>128</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>128</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>128</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>128</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>128</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>128</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>128</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>128</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>128</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>128</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>128</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>128</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>128</v>
       </c>
@@ -7151,9 +7151,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>131</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>131</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>131</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>131</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>131</v>
       </c>
@@ -7346,9 +7346,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>857.83069999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>805.30949999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>805.30949999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>556.43349999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -7810,7 +7810,7 @@
         <v>6360.8798999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>5844.5888000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -7964,7 +7964,7 @@
         <v>5758.0366000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>5220.0447999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>5220.0447999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -8195,7 +8195,7 @@
         <v>3877.0077000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>3326.8465000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>3755.8728999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -8426,7 +8426,7 @@
         <v>2446.6104999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -8503,7 +8503,7 @@
         <v>2360.2145</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -8580,7 +8580,7 @@
         <v>2360.2145</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>3700.9425000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>1103.3389999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>3538.2548000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
@@ -8888,7 +8888,7 @@
         <v>157.9794</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>229.08629999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>229.08629999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -9119,7 +9119,7 @@
         <v>308.8956</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>2428.4416999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>89</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>2856.1984000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>90</v>
       </c>
@@ -9350,7 +9350,7 @@
         <v>2034.5162</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>1880.6876999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>1880.6876999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -9581,7 +9581,7 @@
         <v>2304.2213000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
@@ -9658,7 +9658,7 @@
         <v>1418.8416</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>90</v>
       </c>
@@ -9735,7 +9735,7 @@
         <v>1769.1315999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
@@ -9812,7 +9812,7 @@
         <v>4167.3869999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -9889,7 +9889,7 @@
         <v>3875.0300999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
@@ -9966,7 +9966,7 @@
         <v>3875.0300999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>3443.2374</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>2134.3492999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>91</v>
       </c>
@@ -10208,9 +10208,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -10236,7 +10236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -10262,7 +10262,7 @@
         <v>12944.397499999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -10288,7 +10288,7 @@
         <v>10381.2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>8654.8163000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -10340,7 +10340,7 @@
         <v>8797.1162999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>8797.1162999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -10392,7 +10392,7 @@
         <v>8683.2186000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -10418,7 +10418,7 @@
         <v>145171.73430000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -10444,7 +10444,7 @@
         <v>132654.20480000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>156266.19940000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>145500.89319999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>145500.89319999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -10548,7 +10548,7 @@
         <v>137239.86230000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -10574,7 +10574,7 @@
         <v>83.248099999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>16.051100000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>6044.6253999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -10652,7 +10652,7 @@
         <v>5444.3622999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -10678,7 +10678,7 @@
         <v>6519.0657000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>6080.5290000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>6080.5290000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>6039.4964</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -10782,7 +10782,7 @@
         <v>6669.7326000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -10808,7 +10808,7 @@
         <v>6240.1718000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -10834,7 +10834,7 @@
         <v>6240.1718000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -10860,7 +10860,7 @@
         <v>6358.1406999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -10886,7 +10886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -10912,7 +10912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>67710.320099999997</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -10964,7 +10964,7 @@
         <v>69101.584199999998</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>69101.584199999998</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -11016,7 +11016,7 @@
         <v>64966.260199999997</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -11042,7 +11042,7 @@
         <v>68543.796300000002</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -11068,7 +11068,7 @@
         <v>63869.9185</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -11094,7 +11094,7 @@
         <v>148.74340000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>74.371700000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -11146,7 +11146,7 @@
         <v>4863.0127000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -11181,16 +11181,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -11225,7 +11225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -11260,7 +11260,7 @@
         <v>307616.19189999998</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -11295,7 +11295,7 @@
         <v>524632.15249999997</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -11330,7 +11330,7 @@
         <v>1024974.6192</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>1173483.1459999999</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>1173483.1459999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -11435,7 +11435,7 @@
         <v>819916.6666</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -11470,7 +11470,7 @@
         <v>281497.3714</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>490165.98930000002</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -11540,7 +11540,7 @@
         <v>1246703.7124999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -11575,7 +11575,7 @@
         <v>1068678.895</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -11610,7 +11610,7 @@
         <v>1068678.895</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>722260.39839999995</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>623.05989999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -11715,7 +11715,7 @@
         <v>564.72260000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -11750,7 +11750,7 @@
         <v>4661.1570000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -11785,7 +11785,7 @@
         <v>2683.2386000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -11820,7 +11820,7 @@
         <v>3422.8395</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -11855,7 +11855,7 @@
         <v>2774.8618000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -11890,7 +11890,7 @@
         <v>2774.8618000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>2316.9856</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -11960,7 +11960,7 @@
         <v>18613.923999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -11995,7 +11995,7 @@
         <v>14893.258400000001</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -12030,7 +12030,7 @@
         <v>14893.258400000001</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -12065,7 +12065,7 @@
         <v>11830.2752</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -12100,7 +12100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -12170,7 +12170,7 @@
         <v>256042.7807</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>288000</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -12240,7 +12240,7 @@
         <v>288000</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>201409.69159999999</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>861052.63150000002</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -12345,7 +12345,7 @@
         <v>308163.26530000003</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -12380,7 +12380,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -12415,7 +12415,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -12450,7 +12450,7 @@
         <v>65217.391300000003</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -12496,9 +12496,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -12548,7 +12548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -12598,7 +12598,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -12698,7 +12698,7 @@
         <v>1.44E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -12748,7 +12748,7 @@
         <v>1.44E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
@@ -12798,7 +12798,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -12848,7 +12848,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -12909,9 +12909,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -12925,7 +12925,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -12939,7 +12939,7 @@
         <v>11526.643599999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -12953,7 +12953,7 @@
         <v>11533.2065</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
@@ -12967,7 +12967,7 @@
         <v>11533.2065</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -12981,7 +12981,7 @@
         <v>11334.2238</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>10586.8572</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -13020,9 +13020,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -13072,7 +13072,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -13122,7 +13122,7 @@
         <v>82756.125799999994</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -13172,7 +13172,7 @@
         <v>82756.125799999994</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>82756.125799999994</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>76</v>
       </c>
@@ -13272,7 +13272,7 @@
         <v>82756.125799999994</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -13322,7 +13322,7 @@
         <v>83583.443400000004</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -13372,7 +13372,7 @@
         <v>82756.125799999994</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>19820.227599999998</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -13472,7 +13472,7 @@
         <v>19820.227599999998</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>77</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>19820.227599999998</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -13572,7 +13572,7 @@
         <v>19820.227599999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>77</v>
       </c>
@@ -13622,7 +13622,7 @@
         <v>19612.4771</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>19820.227599999998</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -13722,7 +13722,7 @@
         <v>126607.9892</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
@@ -13772,7 +13772,7 @@
         <v>126607.9892</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -13822,7 +13822,7 @@
         <v>126607.9892</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -13872,7 +13872,7 @@
         <v>126607.9892</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
@@ -13922,7 +13922,7 @@
         <v>129196.67479999999</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
@@ -13983,9 +13983,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -14032,7 +14032,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -14079,7 +14079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -14126,7 +14126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -14173,7 +14173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>76</v>
       </c>
@@ -14220,7 +14220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -14267,7 +14267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -14314,7 +14314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -14361,7 +14361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -14408,7 +14408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>76</v>
       </c>
@@ -14502,7 +14502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -14549,7 +14549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -14596,7 +14596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
@@ -14643,7 +14643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
@@ -14690,7 +14690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -14737,7 +14737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -14784,7 +14784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -14831,7 +14831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -14878,7 +14878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -14925,7 +14925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -14972,7 +14972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>76</v>
       </c>
@@ -15019,7 +15019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -15066,7 +15066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -15113,7 +15113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -15160,7 +15160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -15207,7 +15207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -15254,7 +15254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -15301,7 +15301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
@@ -15348,7 +15348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
@@ -15395,7 +15395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -15442,7 +15442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
@@ -15489,7 +15489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -15536,7 +15536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -15583,7 +15583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -15630,7 +15630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
@@ -15677,7 +15677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -15724,7 +15724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>77</v>
       </c>
@@ -15771,7 +15771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>77</v>
       </c>
@@ -15818,7 +15818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>77</v>
       </c>
@@ -15865,7 +15865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>77</v>
       </c>
@@ -15959,7 +15959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>77</v>
       </c>
@@ -16006,7 +16006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
@@ -16053,7 +16053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>77</v>
       </c>
@@ -16100,7 +16100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>77</v>
       </c>
@@ -16147,7 +16147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
@@ -16194,7 +16194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>77</v>
       </c>
@@ -16241,7 +16241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>77</v>
       </c>
@@ -16288,7 +16288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>77</v>
       </c>
@@ -16335,7 +16335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
@@ -16382,7 +16382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>77</v>
       </c>
@@ -16429,7 +16429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -16476,7 +16476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
@@ -16523,7 +16523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>77</v>
       </c>
@@ -16570,7 +16570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>78</v>
       </c>
@@ -16617,7 +16617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>78</v>
       </c>
@@ -16664,7 +16664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>78</v>
       </c>
@@ -16711,7 +16711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>78</v>
       </c>
@@ -16758,7 +16758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>78</v>
       </c>
@@ -16805,7 +16805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>78</v>
       </c>
@@ -16852,7 +16852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>78</v>
       </c>
@@ -16899,7 +16899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
@@ -16946,7 +16946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>78</v>
       </c>
@@ -16993,7 +16993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>78</v>
       </c>
@@ -17040,7 +17040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -17087,7 +17087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>78</v>
       </c>
@@ -17134,7 +17134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
@@ -17181,7 +17181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>78</v>
       </c>
@@ -17228,7 +17228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>78</v>
       </c>
@@ -17275,7 +17275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>78</v>
       </c>
@@ -17322,7 +17322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -17369,7 +17369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -17416,7 +17416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -17463,7 +17463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -17510,7 +17510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
@@ -17557,7 +17557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
@@ -17604,7 +17604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
@@ -17651,7 +17651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -17698,7 +17698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -17745,7 +17745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -17792,7 +17792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>78</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>78</v>
       </c>
@@ -17886,7 +17886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>78</v>
       </c>
@@ -17933,7 +17933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>78</v>
       </c>
@@ -17980,7 +17980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>78</v>
       </c>
@@ -18027,7 +18027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>78</v>
       </c>
@@ -18074,7 +18074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>78</v>
       </c>
@@ -18121,7 +18121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>78</v>
       </c>
@@ -18168,7 +18168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>78</v>
       </c>
@@ -18215,7 +18215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>78</v>
       </c>
@@ -18273,9 +18273,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -18349,7 +18349,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -18423,7 +18423,7 @@
         <v>857.83069999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -18497,7 +18497,7 @@
         <v>805.30949999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -18571,7 +18571,7 @@
         <v>805.30949999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -18645,7 +18645,7 @@
         <v>556.43349999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -18719,7 +18719,7 @@
         <v>6360.8798999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -18793,7 +18793,7 @@
         <v>5844.5888000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -18867,7 +18867,7 @@
         <v>5758.0366000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -18941,7 +18941,7 @@
         <v>5220.0447999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -19015,7 +19015,7 @@
         <v>5220.0447999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -19089,7 +19089,7 @@
         <v>3877.0077000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
@@ -19163,7 +19163,7 @@
         <v>3326.8465000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -19237,7 +19237,7 @@
         <v>3755.8728999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -19311,7 +19311,7 @@
         <v>2446.6104999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -19385,7 +19385,7 @@
         <v>2360.2145</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -19459,7 +19459,7 @@
         <v>2360.2145</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -19533,7 +19533,7 @@
         <v>3700.9425000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -19607,7 +19607,7 @@
         <v>1103.3389999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -19681,7 +19681,7 @@
         <v>3538.2548000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
@@ -19755,7 +19755,7 @@
         <v>157.9794</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
@@ -19829,7 +19829,7 @@
         <v>229.08629999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
@@ -19903,7 +19903,7 @@
         <v>229.08629999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -19977,7 +19977,7 @@
         <v>308.8956</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
@@ -20051,7 +20051,7 @@
         <v>2428.4416999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>89</v>
       </c>
@@ -20125,7 +20125,7 @@
         <v>2856.1984000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>90</v>
       </c>
@@ -20199,7 +20199,7 @@
         <v>2034.5162</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
@@ -20273,7 +20273,7 @@
         <v>1880.6876999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
@@ -20347,7 +20347,7 @@
         <v>1880.6876999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -20421,7 +20421,7 @@
         <v>2304.2213000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
@@ -20495,7 +20495,7 @@
         <v>1418.8416</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>90</v>
       </c>
@@ -20569,7 +20569,7 @@
         <v>1769.1315999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
@@ -20643,7 +20643,7 @@
         <v>4167.3869999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -20717,7 +20717,7 @@
         <v>3875.0300999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
@@ -20791,7 +20791,7 @@
         <v>3875.0300999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -20865,7 +20865,7 @@
         <v>3443.2374</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
@@ -20939,7 +20939,7 @@
         <v>2134.3492999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>91</v>
       </c>
@@ -21022,11 +21022,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -21061,7 +21071,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -21094,7 +21104,7 @@
         <v>0.29420000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -21127,7 +21137,7 @@
         <v>0.19769999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -21160,7 +21170,7 @@
         <v>0.19769999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -21193,7 +21203,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -21226,7 +21236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -21259,7 +21269,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -21288,7 +21298,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -21317,7 +21327,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -21346,7 +21356,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -21375,7 +21385,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -21404,7 +21414,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -21433,7 +21443,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -21468,7 +21478,7 @@
         <v>1.1194999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -21503,7 +21513,7 @@
         <v>1.3832</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -21538,7 +21548,7 @@
         <v>1.3832</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>111</v>
       </c>
@@ -21573,7 +21583,7 @@
         <v>0.64649999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -21608,7 +21618,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Added important KPIs to Purchasing section| updated the map with correct data, changed the map so that it shows the correct contry| added graps and plots to Operations mixing and bottling section
</commit_message>
<xml_diff>
--- a/Data/MAIN_DATA_FILE.xlsx
+++ b/Data/MAIN_DATA_FILE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andris\Desktop\PEI_LD4_Streamlit_Dash_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D447809B-BAD0-4A45-86E1-9D067B8AE267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48EB8DC-6F2D-43C0-9274-9DDAF57956B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="914" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="132">
   <si>
     <t>Component</t>
   </si>
@@ -10204,971 +10204,1088 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>0.94140000000000001</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>3.1099999999999999E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>19.3505</v>
       </c>
       <c r="F2" s="3">
         <v>19.3505</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
+        <v>19.3505</v>
+      </c>
+      <c r="H2" s="1">
         <v>160776.1067</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>12944.397499999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>0.94820000000000004</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>10.6471</v>
       </c>
       <c r="F3" s="3">
         <v>10.6471</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
+        <v>10.6471</v>
+      </c>
+      <c r="H3" s="1">
         <v>149105.82070000001</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>10381.2019</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
         <v>-2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>0.89259999999999995</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5.7152000000000003</v>
       </c>
       <c r="F4" s="3">
         <v>5.7152000000000003</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
+        <v>5.7152000000000003</v>
+      </c>
+      <c r="H4" s="1">
         <v>154869.9504</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>8654.8163000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
         <v>-1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>0.89180000000000004</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>3.3300000000000003E-2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5.1639999999999997</v>
       </c>
       <c r="F5" s="3">
         <v>5.1639999999999997</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3">
+        <v>5.1639999999999997</v>
+      </c>
+      <c r="H5" s="1">
         <v>160052.15400000001</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>8797.1162999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.89180000000000004</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>3.3300000000000003E-2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5.1639999999999997</v>
       </c>
       <c r="F6" s="3">
         <v>5.1639999999999997</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="3">
+        <v>5.1639999999999997</v>
+      </c>
+      <c r="H6" s="1">
         <v>160052.15400000001</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>8797.1162999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>0.89229999999999998</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>3.5299999999999998E-2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>6.9626999999999999</v>
       </c>
       <c r="F7" s="3">
         <v>6.9626999999999999</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
+        <v>6.9626999999999999</v>
+      </c>
+      <c r="H7" s="1">
         <v>151176.35500000001</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>8683.2186000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>0.92169999999999996</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>3.2300000000000002E-2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>20.3079</v>
       </c>
       <c r="F8" s="3">
         <v>20.3079</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
+        <v>20.3079</v>
+      </c>
+      <c r="H8" s="1">
         <v>316087.81670000002</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>145171.73430000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>0.9335</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>3.0300000000000001E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>10.850199999999999</v>
       </c>
       <c r="F9" s="3">
         <v>10.850199999999999</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
+        <v>10.850199999999999</v>
+      </c>
+      <c r="H9" s="1">
         <v>291664.52860000002</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>132654.20480000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1">
         <v>-2</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>0.88680000000000003</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>0.04</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4.8449</v>
       </c>
       <c r="F10" s="3">
         <v>4.8449</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
+        <v>4.8449</v>
+      </c>
+      <c r="H10" s="1">
         <v>332034.72970000003</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>156266.19940000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
         <v>-1</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>0.88880000000000003</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5.2510000000000003</v>
       </c>
       <c r="F11" s="3">
         <v>5.2510000000000003</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
+        <v>5.2510000000000003</v>
+      </c>
+      <c r="H11" s="1">
         <v>308801.2769</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>145500.89319999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
         <v>0.88880000000000003</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>5.2510000000000003</v>
       </c>
       <c r="F12" s="3">
         <v>5.2510000000000003</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
+        <v>5.2510000000000003</v>
+      </c>
+      <c r="H12" s="1">
         <v>308801.2769</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>145500.89319999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>0.93069999999999997</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>4.2299999999999997E-2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>7.2817999999999996</v>
       </c>
       <c r="F13" s="3">
         <v>7.2817999999999996</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
+        <v>7.2817999999999996</v>
+      </c>
+      <c r="H13" s="1">
         <v>290067.41279999999</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>137239.86230000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.29010000000000002</v>
+      <c r="E14" s="2">
+        <v>0</v>
       </c>
       <c r="F14" s="3">
         <v>0.29010000000000002</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
+        <v>0.29010000000000002</v>
+      </c>
+      <c r="H14" s="1">
         <v>951.61090000000002</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>83.248099999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>5.8000000000000003E-2</v>
+      <c r="E15" s="2">
+        <v>0</v>
       </c>
       <c r="F15" s="3">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H15" s="1">
         <v>173.46270000000001</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>16.051100000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>3.1899999999999998E-2</v>
-      </c>
-      <c r="E16" s="3">
-        <v>3.5103</v>
       </c>
       <c r="F16" s="3">
         <v>3.5103</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
+        <v>3.5103</v>
+      </c>
+      <c r="H16" s="1">
         <v>68941.764500000005</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>6044.6253999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>0.98939999999999995</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>2.7E-2</v>
-      </c>
-      <c r="E17" s="3">
-        <v>5.1059999999999999</v>
       </c>
       <c r="F17" s="3">
         <v>5.1059999999999999</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="3">
+        <v>5.1059999999999999</v>
+      </c>
+      <c r="H17" s="1">
         <v>58109.564299999998</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>5444.3622999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
         <v>-2</v>
       </c>
-      <c r="C18" s="2">
+      <c r="D18" s="2">
         <v>0.88449999999999995</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>8.0600000000000005E-2</v>
-      </c>
-      <c r="E18" s="3">
-        <v>4.6997999999999998</v>
       </c>
       <c r="F18" s="3">
         <v>4.6997999999999998</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="3">
+        <v>4.6997999999999998</v>
+      </c>
+      <c r="H18" s="1">
         <v>55500.1878</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>6519.0657000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1">
         <v>-1</v>
       </c>
-      <c r="C19" s="2">
+      <c r="D19" s="2">
         <v>0.89339999999999997</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>7.9100000000000004E-2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>5.2510000000000003</v>
       </c>
       <c r="F19" s="3">
         <v>5.2510000000000003</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="3">
+        <v>5.2510000000000003</v>
+      </c>
+      <c r="H19" s="1">
         <v>50446.207199999997</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>6080.5290000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
         <v>0.89339999999999997</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="2">
         <v>7.9100000000000004E-2</v>
-      </c>
-      <c r="E20" s="3">
-        <v>5.2510000000000003</v>
       </c>
       <c r="F20" s="3">
         <v>5.2510000000000003</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="3">
+        <v>5.2510000000000003</v>
+      </c>
+      <c r="H20" s="1">
         <v>50446.207199999997</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>6080.5290000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="2">
+      <c r="D21" s="2">
         <v>0.92769999999999997</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E21" s="2">
         <v>5.62E-2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>6.0632999999999999</v>
       </c>
       <c r="F21" s="3">
         <v>6.0632999999999999</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="3">
+        <v>6.0632999999999999</v>
+      </c>
+      <c r="H21" s="1">
         <v>60391.344599999997</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>6039.4964</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1">
         <v>-2</v>
       </c>
-      <c r="C22" s="2">
+      <c r="D22" s="2">
         <v>0.84860000000000002</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <v>2.5100000000000001E-2</v>
-      </c>
-      <c r="E22" s="3">
-        <v>4.5837000000000003</v>
       </c>
       <c r="F22" s="3">
         <v>4.5837000000000003</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="3">
+        <v>4.5837000000000003</v>
+      </c>
+      <c r="H22" s="1">
         <v>96580.207899999994</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>6669.7326000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1">
         <v>-1</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D23" s="2">
         <v>0.84230000000000005</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E23" s="2">
         <v>1.77E-2</v>
-      </c>
-      <c r="E23" s="3">
-        <v>5.1639999999999997</v>
       </c>
       <c r="F23" s="3">
         <v>5.1639999999999997</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="3">
+        <v>5.1639999999999997</v>
+      </c>
+      <c r="H23" s="1">
         <v>87284.942299999995</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>6240.1718000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
         <v>0.84230000000000005</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E24" s="2">
         <v>1.77E-2</v>
-      </c>
-      <c r="E24" s="3">
-        <v>5.1639999999999997</v>
       </c>
       <c r="F24" s="3">
         <v>5.1639999999999997</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="3">
+        <v>5.1639999999999997</v>
+      </c>
+      <c r="H24" s="1">
         <v>87284.942299999995</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>6240.1718000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="2">
+      <c r="D25" s="2">
         <v>0.92820000000000003</v>
       </c>
-      <c r="D25" s="2">
+      <c r="E25" s="2">
         <v>1.43E-2</v>
-      </c>
-      <c r="E25" s="3">
-        <v>6.3243999999999998</v>
       </c>
       <c r="F25" s="3">
         <v>6.3243999999999998</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="3">
+        <v>6.3243999999999998</v>
+      </c>
+      <c r="H25" s="1">
         <v>85615.340200000006</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>6358.1406999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1">
         <v>2</v>
       </c>
-      <c r="C26" s="2">
+      <c r="D26" s="2">
         <v>1</v>
       </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>0</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="3">
         <v>0</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1">
         <v>3</v>
       </c>
-      <c r="C27" s="2">
+      <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>0</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="3">
         <v>0</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1">
         <v>-2</v>
       </c>
-      <c r="C28" s="2">
+      <c r="D28" s="2">
         <v>0.97609999999999997</v>
       </c>
-      <c r="D28" s="2">
+      <c r="E28" s="2">
         <v>1.06E-2</v>
-      </c>
-      <c r="E28" s="3">
-        <v>5.4250999999999996</v>
       </c>
       <c r="F28" s="3">
         <v>5.4250999999999996</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="3">
+        <v>5.4250999999999996</v>
+      </c>
+      <c r="H28" s="1">
         <v>721543.18779999996</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>67710.320099999997</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1">
         <v>-1</v>
       </c>
-      <c r="C29" s="2">
+      <c r="D29" s="2">
         <v>0.98219999999999996</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E29" s="2">
         <v>1.34E-2</v>
-      </c>
-      <c r="E29" s="3">
-        <v>4.9318999999999997</v>
       </c>
       <c r="F29" s="3">
         <v>4.9318999999999997</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="3">
+        <v>4.9318999999999997</v>
+      </c>
+      <c r="H29" s="1">
         <v>737682.56160000002</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>69101.584199999998</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
         <v>0.98219999999999996</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" s="2">
         <v>1.34E-2</v>
-      </c>
-      <c r="E30" s="3">
-        <v>4.9318999999999997</v>
       </c>
       <c r="F30" s="3">
         <v>4.9318999999999997</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="3">
+        <v>4.9318999999999997</v>
+      </c>
+      <c r="H30" s="1">
         <v>737682.56160000002</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>69101.584199999998</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="2">
+      <c r="D31" s="2">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D31" s="2">
+      <c r="E31" s="2">
         <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="E31" s="3">
-        <v>6.5854999999999997</v>
       </c>
       <c r="F31" s="3">
         <v>6.5854999999999997</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="3">
+        <v>6.5854999999999997</v>
+      </c>
+      <c r="H31" s="1">
         <v>689302.90830000001</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>64966.260199999997</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1">
         <v>2</v>
       </c>
-      <c r="C32" s="2">
+      <c r="D32" s="2">
         <v>1</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E32" s="2">
         <v>1.83E-2</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1.6536</v>
       </c>
       <c r="F32" s="3">
         <v>1.6536</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="3">
+        <v>1.6536</v>
+      </c>
+      <c r="H32" s="1">
         <v>738763.45259999996</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>68543.796300000002</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1">
         <v>3</v>
       </c>
-      <c r="C33" s="2">
+      <c r="D33" s="2">
         <v>0.98670000000000002</v>
       </c>
-      <c r="D33" s="2">
+      <c r="E33" s="2">
         <v>1.32E-2</v>
-      </c>
-      <c r="E33" s="3">
-        <v>4.2645999999999997</v>
       </c>
       <c r="F33" s="3">
         <v>4.2645999999999997</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="3">
+        <v>4.2645999999999997</v>
+      </c>
+      <c r="H33" s="1">
         <v>682471.19050000003</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>63869.9185</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="1">
         <v>2</v>
       </c>
-      <c r="C34" s="2">
+      <c r="D34" s="2">
         <v>1</v>
       </c>
-      <c r="D34" s="2">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0.11600000000000001</v>
+      <c r="E34" s="2">
+        <v>0</v>
       </c>
       <c r="F34" s="3">
         <v>0.11600000000000001</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="H34" s="1">
         <v>4899.8154999999997</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>148.74340000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1">
         <v>3</v>
       </c>
-      <c r="C35" s="2">
+      <c r="D35" s="2">
         <v>0.5</v>
       </c>
-      <c r="D35" s="2">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
-        <v>5.8000000000000003E-2</v>
+      <c r="E35" s="2">
+        <v>0</v>
       </c>
       <c r="F35" s="3">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H35" s="1">
         <v>2432.6749</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>74.371700000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="1">
         <v>2</v>
       </c>
-      <c r="C36" s="2">
+      <c r="D36" s="2">
         <v>0.89</v>
       </c>
-      <c r="D36" s="2">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3">
-        <v>1.3345</v>
+      <c r="E36" s="2">
+        <v>0</v>
       </c>
       <c r="F36" s="3">
         <v>1.3345</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="3">
+        <v>1.3345</v>
+      </c>
+      <c r="H36" s="1">
         <v>100495.26</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>4863.0127000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="1">
         <v>3</v>
       </c>
-      <c r="C37" s="2">
+      <c r="D37" s="2">
         <v>0.85540000000000005</v>
       </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
-        <v>2.4079000000000002</v>
+      <c r="E37" s="2">
+        <v>0</v>
       </c>
       <c r="F37" s="3">
         <v>2.4079000000000002</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="3">
+        <v>2.4079000000000002</v>
+      </c>
+      <c r="H37" s="1">
         <v>83807.683199999999</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>4323.6575000000003</v>
       </c>
     </row>
@@ -12494,9 +12611,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" customWidth="1"/>
+    <col min="14" max="14" width="27.5546875" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -12907,9 +13036,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -21022,8 +21157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>